<commit_message>
karthik chnages in assert
</commit_message>
<xml_diff>
--- a/Project/testData/ELCData.xlsx
+++ b/Project/testData/ELCData.xlsx
@@ -397,14 +397,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
-        <v/>
+        <v>Cars</v>
       </c>
       <c r="B1" t="str">
         <v/>
@@ -415,9 +415,23 @@
         <v>Puzzles</v>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v>https://www.elc.co.uk/brands/paw-patrol</v>
+      </c>
+      <c r="B7" t="str">
+        <v>Narrow Your Results</v>
+      </c>
+      <c r="C7" t="str">
+        <v>Available to pick up for FREE from our stores within 30 minutes.</v>
+      </c>
+      <c r="D7" t="str">
+        <v>Add to Basket</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:B2"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:D7"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>